<commit_message>
All work done for image to table convertion . ready for server
</commit_message>
<xml_diff>
--- a/xlsl_file/IMG_20240520_162440table.xlsx
+++ b/xlsl_file/IMG_20240520_162440table.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
-    <t>Question No</t>
+    <t>Question No.</t>
   </si>
   <si>
     <t>Marks</t>
@@ -61,7 +61,7 @@
     <t>08</t>
   </si>
   <si>
-    <t>17.5</t>
+    <t>175</t>
   </si>
   <si>
     <t>09</t>
@@ -426,7 +426,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>